<commit_message>
updates to flow deliverable
</commit_message>
<xml_diff>
--- a/2 - Flow output Excel files - working drafts/Data Output 07_31_2019/Offsets and Clip times 07_31_2019.xlsx
+++ b/2 - Flow output Excel files - working drafts/Data Output 07_31_2019/Offsets and Clip times 07_31_2019.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="9330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="9330" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Offsets" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="105">
   <si>
     <t>Site</t>
   </si>
@@ -324,70 +324,34 @@
     <t>Sensor failure, was replaced 7/16</t>
   </si>
   <si>
-    <t>Demobed 7/12</t>
-  </si>
-  <si>
-    <t>Another high flow event 7/22. Smaller but longer duration flow event 7/10</t>
-  </si>
-  <si>
-    <t>Several very large flows in June but no reason to remove them. Any other data to discount/corroborate these?</t>
-  </si>
-  <si>
-    <t>New probe installed. High flow event 7/16</t>
-  </si>
-  <si>
-    <t>High flow event 7/16</t>
-  </si>
-  <si>
-    <t>High flow event 7/16, possible stormflow? Also high flow event 7/22 (same as SDR-097?)</t>
-  </si>
-  <si>
-    <t>Very high flow event 7/16</t>
-  </si>
-  <si>
-    <t>High flow events 7/3 and 7/11</t>
-  </si>
-  <si>
-    <t>High flow event 7/19. Mostly no flow now?</t>
-  </si>
-  <si>
-    <t>None. Looks like going dry</t>
-  </si>
-  <si>
-    <t>High flow event 7/18</t>
-  </si>
-  <si>
-    <t>High flow event 7/16 followed by series of higher flows</t>
-  </si>
-  <si>
-    <t>Early May flow should have been clipped out</t>
-  </si>
-  <si>
-    <t>Clear weekday flows pattern, then no flow on weekends. Data stops at 7/19? Where's the rest of the data?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clear weekday flows pattern, then no flow on weekends. </t>
-  </si>
-  <si>
-    <t>storm clips during 6/17 and 6/21 not needed</t>
-  </si>
-  <si>
-    <t>level spike on 7/15 same day as manual download</t>
-  </si>
-  <si>
-    <t>data drop out 7/2, 7/11, 7/13, 7/14, 7/15, 7/17, 7/20</t>
-  </si>
-  <si>
-    <t>data drop outs 6/2, 7/6, 7/9, 7/10, 7/11, 7/14, 7/17, 7/20, 7/22</t>
-  </si>
-  <si>
-    <t>data drop outs 7/1, 7/3, 7/9, 7/19, 7/20, 7/22</t>
-  </si>
-  <si>
     <t>Data Dropout</t>
   </si>
   <si>
     <t>Data gap. Possible battery failure.</t>
+  </si>
+  <si>
+    <t>Data dropouts</t>
+  </si>
+  <si>
+    <t>weird spikes in flow</t>
+  </si>
+  <si>
+    <t>Data gaps and some weird spikes in flow</t>
+  </si>
+  <si>
+    <t>Some high flow in late july</t>
+  </si>
+  <si>
+    <t>Still some high flow late in July</t>
+  </si>
+  <si>
+    <t>Data stops at 7/29ish? Where's the rest of the data?</t>
+  </si>
+  <si>
+    <t>Data stops at 7/30ish? Where's the rest of the data?</t>
+  </si>
+  <si>
+    <t>Demobed 7/12. Deliverable ends at end of day 7/12.</t>
   </si>
 </sst>
 </file>
@@ -2626,7 +2590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFC1368"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A371" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B387" sqref="B387"/>
     </sheetView>
@@ -2828,7 +2792,7 @@
         <v>43647.659722222219</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4034,7 +3998,7 @@
         <v>43668.552083333336</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="97" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -25247,11 +25211,11 @@
   </sheetPr>
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -25395,7 +25359,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C15" s="11"/>
     </row>
@@ -25404,7 +25368,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C16" s="11"/>
     </row>
@@ -25417,12 +25381,12 @@
       </c>
       <c r="C17" s="11"/>
     </row>
-    <row r="18" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C18" s="11"/>
     </row>
@@ -25431,7 +25395,7 @@
         <v>41</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C19" s="11"/>
     </row>
@@ -25440,16 +25404,16 @@
         <v>13</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C20" s="11"/>
     </row>
-    <row r="21" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C21" s="11"/>
     </row>
@@ -25458,7 +25422,7 @@
         <v>14</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C22" s="11"/>
     </row>
@@ -25467,7 +25431,7 @@
         <v>15</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C23" s="11"/>
     </row>
@@ -25476,7 +25440,7 @@
         <v>16</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C24" s="11"/>
     </row>
@@ -25485,7 +25449,7 @@
         <v>32</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C25" s="11"/>
     </row>
@@ -25494,7 +25458,7 @@
         <v>17</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C26" s="11"/>
     </row>
@@ -25503,7 +25467,7 @@
         <v>33</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C27" s="11"/>
     </row>
@@ -25512,7 +25476,7 @@
         <v>34</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C28" s="11"/>
     </row>
@@ -25530,7 +25494,7 @@
         <v>36</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="C30" s="11"/>
     </row>
@@ -25539,7 +25503,7 @@
         <v>37</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="C31" s="11"/>
     </row>
@@ -25548,7 +25512,7 @@
         <v>38</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="C32" s="11"/>
     </row>
@@ -25566,7 +25530,7 @@
         <v>44</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="C34" s="11"/>
     </row>
@@ -25575,7 +25539,7 @@
         <v>45</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="C35" s="11"/>
     </row>
@@ -25584,7 +25548,7 @@
         <v>46</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C36" s="11"/>
     </row>
@@ -25593,7 +25557,7 @@
         <v>18</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="C37" s="11"/>
     </row>
@@ -25602,7 +25566,7 @@
         <v>26</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="C38" s="11"/>
     </row>
@@ -25611,7 +25575,7 @@
         <v>19</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C39" s="11"/>
     </row>
@@ -25620,7 +25584,7 @@
         <v>20</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="C40" s="11"/>
     </row>

</xml_diff>

<commit_message>
last update on 8/7/19
</commit_message>
<xml_diff>
--- a/2 - Flow output Excel files - working drafts/Data Output 07_31_2019/Offsets and Clip times 07_31_2019.xlsx
+++ b/2 - Flow output Excel files - working drafts/Data Output 07_31_2019/Offsets and Clip times 07_31_2019.xlsx
@@ -548,7 +548,7 @@
         <xdr:cNvPr id="2" name="EsriDoNotEdit">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25536,7 +25536,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added pic viewer to main script
</commit_message>
<xml_diff>
--- a/2 - Flow output Excel files - working drafts/Data Output 07_31_2019/Offsets and Clip times 07_31_2019.xlsx
+++ b/2 - Flow output Excel files - working drafts/Data Output 07_31_2019/Offsets and Clip times 07_31_2019.xlsx
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Clips!$A$1:$E$465</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Data Deliverable Notes'!$A$1:$C$41</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Offsets!$A$1:$G$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Offsets!$A$1:$G$67</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1156" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="125">
   <si>
     <t>Site</t>
   </si>
@@ -929,13 +929,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G202"/>
+  <dimension ref="A1:G203"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B51" sqref="B51"/>
+      <selection pane="bottomRight" activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1692,11 +1692,11 @@
       <c r="B49" s="1">
         <v>43619.447916666664</v>
       </c>
-      <c r="C49" s="1">
-        <v>43647.489583333336</v>
+      <c r="C49" s="8">
+        <v>43633.09375</v>
       </c>
       <c r="D49" s="7">
-        <v>1</v>
+        <v>1.7</v>
       </c>
       <c r="E49" s="14">
         <v>0.5</v>
@@ -1710,10 +1710,10 @@
         <v>45</v>
       </c>
       <c r="B50" s="8">
-        <v>43647.489583333336</v>
-      </c>
-      <c r="C50" s="8">
-        <v>43677.996527777781</v>
+        <v>43633.097222222219</v>
+      </c>
+      <c r="C50" s="1">
+        <v>43647.486111111109</v>
       </c>
       <c r="D50" s="7">
         <v>1.8</v>
@@ -1726,16 +1726,44 @@
       </c>
     </row>
     <row r="51" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="5"/>
+      <c r="A51" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" s="8">
+        <v>43647.489583333336</v>
+      </c>
+      <c r="C51" s="8">
+        <v>43661.625</v>
+      </c>
+      <c r="D51" s="7">
+        <v>2.6</v>
+      </c>
+      <c r="E51" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F51" s="5" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="52" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="5"/>
+      <c r="A52" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B52" s="8">
+        <v>43661.628472222219</v>
+      </c>
+      <c r="C52" s="8">
+        <v>43677.996527777781</v>
+      </c>
+      <c r="D52" s="7">
+        <v>0.65</v>
+      </c>
+      <c r="E52" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F52" s="5" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="53" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B53" s="8"/>
@@ -1755,56 +1783,44 @@
       <c r="E55" s="14"/>
       <c r="F55" s="5"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="7" t="s">
-        <v>46</v>
-      </c>
+    <row r="56" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
-      <c r="D56" s="7">
-        <v>0</v>
-      </c>
-      <c r="E56" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="F56" s="5" t="b">
-        <v>1</v>
-      </c>
+      <c r="E56" s="14"/>
+      <c r="F56" s="5"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B57" s="8">
-        <v>43592.649305555598</v>
-      </c>
-      <c r="C57" s="8">
-        <v>43594.708333333299</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
       <c r="D57" s="7">
         <v>0</v>
       </c>
       <c r="E57" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="F57" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" s="8">
+        <v>43592.649305555598</v>
+      </c>
+      <c r="C58" s="8">
+        <v>43594.708333333299</v>
+      </c>
+      <c r="D58" s="7">
         <v>0</v>
       </c>
-      <c r="F57" s="26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>26</v>
-      </c>
-      <c r="B58" s="1">
-        <v>43586</v>
-      </c>
-      <c r="C58" s="1">
-        <v>43592.770833333299</v>
-      </c>
-      <c r="D58">
-        <v>4.25</v>
-      </c>
-      <c r="E58" s="22"/>
+      <c r="E58" s="14">
+        <v>0</v>
+      </c>
       <c r="F58" s="26" t="b">
         <v>1</v>
       </c>
@@ -1814,13 +1830,13 @@
         <v>26</v>
       </c>
       <c r="B59" s="1">
+        <v>43586</v>
+      </c>
+      <c r="C59" s="1">
         <v>43592.770833333299</v>
       </c>
-      <c r="C59" s="1">
-        <v>43593.708333333336</v>
-      </c>
       <c r="D59">
-        <v>3.5</v>
+        <v>4.25</v>
       </c>
       <c r="E59" s="22"/>
       <c r="F59" s="26" t="b">
@@ -1831,9 +1847,16 @@
       <c r="A60" t="s">
         <v>26</v>
       </c>
-      <c r="E60" s="22">
-        <v>0.25</v>
-      </c>
+      <c r="B60" s="1">
+        <v>43592.770833333299</v>
+      </c>
+      <c r="C60" s="1">
+        <v>43593.708333333336</v>
+      </c>
+      <c r="D60">
+        <v>3.5</v>
+      </c>
+      <c r="E60" s="22"/>
       <c r="F60" s="26" t="b">
         <v>1</v>
       </c>
@@ -1842,24 +1865,27 @@
       <c r="A61" t="s">
         <v>26</v>
       </c>
-      <c r="E61" s="14">
+      <c r="E61" s="22">
         <v>0.25</v>
       </c>
-      <c r="F61" s="5" t="b">
+      <c r="F61" s="26" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>19</v>
-      </c>
-      <c r="F62" s="26" t="b">
+        <v>26</v>
+      </c>
+      <c r="E62" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="F62" s="5" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F63" s="26" t="b">
         <v>1</v>
@@ -1867,7 +1893,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F64" s="26" t="b">
         <v>1</v>
@@ -1877,33 +1903,35 @@
       <c r="A65" t="s">
         <v>25</v>
       </c>
-      <c r="F65" s="5" t="s">
-        <v>81</v>
+      <c r="F65" s="26" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
+        <v>25</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>4</v>
       </c>
-      <c r="B66" s="8">
+      <c r="B67" s="8">
         <v>43647.659722222219</v>
       </c>
-      <c r="C66" s="8">
+      <c r="C67" s="8">
         <v>43739</v>
       </c>
-      <c r="D66">
+      <c r="D67">
         <v>-0.15</v>
       </c>
-      <c r="E66"/>
-      <c r="F66" s="26" t="b">
+      <c r="E67"/>
+      <c r="F67" s="26" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B67"/>
-      <c r="C67"/>
-      <c r="E67"/>
-      <c r="F67"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B68"/>
@@ -2715,8 +2743,14 @@
       <c r="E202"/>
       <c r="F202"/>
     </row>
+    <row r="203" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B203"/>
+      <c r="C203"/>
+      <c r="E203"/>
+      <c r="F203"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G66">
+  <autoFilter ref="A1:G67">
     <sortState ref="A2:G58">
       <sortCondition ref="A2:A58"/>
       <sortCondition ref="B2:B58"/>

</xml_diff>

<commit_message>
updated save to Excel Plots
</commit_message>
<xml_diff>
--- a/2 - Flow output Excel files - working drafts/Data Output 07_31_2019/Offsets and Clip times 07_31_2019.xlsx
+++ b/2 - Flow output Excel files - working drafts/Data Output 07_31_2019/Offsets and Clip times 07_31_2019.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="9336"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="9336" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Offsets" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,9 @@
     <sheet name="ESRI_MAPINFO_SHEET" sheetId="4" state="veryHidden" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Clips!$A$1:$E$465</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Clips!$A$1:$E$472</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Data Deliverable Notes'!$A$1:$C$41</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Offsets!$A$1:$G$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Offsets!$A$1:$G$70</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="127">
   <si>
     <t>Site</t>
   </si>
@@ -355,9 +355,6 @@
     <t xml:space="preserve">Clear weekday flows pattern, then no flow on weekends. </t>
   </si>
   <si>
-    <t>level spike on 7/15 same day as manual download</t>
-  </si>
-  <si>
     <t>data drop out 7/2, 7/11, 7/13, 7/14, 7/15, 7/17, 7/20</t>
   </si>
   <si>
@@ -407,6 +404,15 @@
   </si>
   <si>
     <t xml:space="preserve">some drop offs in </t>
+  </si>
+  <si>
+    <t>Bad data-doesn't match with game cam</t>
+  </si>
+  <si>
+    <t>May have been sediment issue</t>
+  </si>
+  <si>
+    <t>level spike on 7/15 same day as manual download. Looks like pattern of higher water temp with the pumping pattern. One period of data (7/9-7/15) was clipped out since it didn't match up with the game cam observations</t>
   </si>
 </sst>
 </file>
@@ -586,7 +592,7 @@
         <xdr:cNvPr id="2" name="EsriDoNotEdit">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -929,13 +935,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G203"/>
+  <dimension ref="A1:G206"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D50" sqref="D50"/>
+      <selection pane="bottomRight" activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1678,12 +1684,8 @@
       <c r="D48" s="7">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E48" s="22">
-        <v>0.5</v>
-      </c>
-      <c r="F48" s="26" t="b">
-        <v>1</v>
-      </c>
+      <c r="E48" s="22"/>
+      <c r="F48" s="26"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
@@ -1698,12 +1700,6 @@
       <c r="D49" s="7">
         <v>1.7</v>
       </c>
-      <c r="E49" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="F49" s="5" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="50" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
@@ -1712,76 +1708,98 @@
       <c r="B50" s="8">
         <v>43633.097222222219</v>
       </c>
-      <c r="C50" s="1">
-        <v>43647.486111111109</v>
+      <c r="C50" s="8">
+        <v>43641.538194444445</v>
       </c>
       <c r="D50" s="7">
         <v>1.8</v>
       </c>
-      <c r="E50" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="F50" s="5" t="b">
-        <v>1</v>
-      </c>
+      <c r="E50" s="14"/>
+      <c r="F50" s="5"/>
     </row>
     <row r="51" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>45</v>
       </c>
       <c r="B51" s="8">
-        <v>43647.489583333336</v>
+        <v>43641.541666666664</v>
       </c>
       <c r="C51" s="8">
-        <v>43661.625</v>
+        <v>43642.052083333336</v>
       </c>
       <c r="D51" s="7">
-        <v>2.6</v>
-      </c>
-      <c r="E51" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="F51" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E51" s="14"/>
+      <c r="F51" s="5"/>
     </row>
     <row r="52" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>45</v>
       </c>
       <c r="B52" s="8">
-        <v>43661.628472222219</v>
+        <v>43642.055555555555</v>
       </c>
       <c r="C52" s="8">
-        <v>43677.996527777781</v>
+        <v>43644.21875</v>
       </c>
       <c r="D52" s="7">
-        <v>0.65</v>
-      </c>
-      <c r="E52" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="F52" s="5" t="b">
+        <v>1.8</v>
+      </c>
+      <c r="E52" s="14"/>
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B53" s="8">
+        <v>43644.21875</v>
+      </c>
+      <c r="C53" s="8">
+        <v>43647.486111111109</v>
+      </c>
+      <c r="D53" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
       <c r="E53" s="14"/>
       <c r="F53" s="5"/>
     </row>
     <row r="54" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="8"/>
-      <c r="C54" s="8"/>
+      <c r="A54" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B54" s="8">
+        <v>43647.489583333336</v>
+      </c>
+      <c r="C54" s="8">
+        <v>43661.625</v>
+      </c>
+      <c r="D54" s="7">
+        <v>2.2000000000000002</v>
+      </c>
       <c r="E54" s="14"/>
       <c r="F54" s="5"/>
     </row>
     <row r="55" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="8"/>
-      <c r="C55" s="8"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="5"/>
+      <c r="A55" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B55" s="8">
+        <v>43661.628472222219</v>
+      </c>
+      <c r="C55" s="8">
+        <v>43677.996527777781</v>
+      </c>
+      <c r="D55" s="7">
+        <v>0.65</v>
+      </c>
+      <c r="E55" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F55" s="5" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="56" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B56" s="8"/>
@@ -1789,84 +1807,54 @@
       <c r="E56" s="14"/>
       <c r="F56" s="5"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="7" t="s">
+    <row r="57" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="8"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="5"/>
+    </row>
+    <row r="58" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="5"/>
+    </row>
+    <row r="59" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="8"/>
+      <c r="C59" s="8"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="5"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="7">
+      <c r="B60" s="8"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="7">
         <v>0</v>
       </c>
-      <c r="E57" s="14">
+      <c r="E60" s="14">
         <v>0.1</v>
       </c>
-      <c r="F57" s="5" t="b">
+      <c r="F60" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="7" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B58" s="8">
+      <c r="B61" s="8">
         <v>43592.649305555598</v>
       </c>
-      <c r="C58" s="8">
+      <c r="C61" s="8">
         <v>43594.708333333299</v>
       </c>
-      <c r="D58" s="7">
+      <c r="D61" s="7">
         <v>0</v>
       </c>
-      <c r="E58" s="14">
+      <c r="E61" s="14">
         <v>0</v>
-      </c>
-      <c r="F58" s="26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>26</v>
-      </c>
-      <c r="B59" s="1">
-        <v>43586</v>
-      </c>
-      <c r="C59" s="1">
-        <v>43592.770833333299</v>
-      </c>
-      <c r="D59">
-        <v>4.25</v>
-      </c>
-      <c r="E59" s="22"/>
-      <c r="F59" s="26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>26</v>
-      </c>
-      <c r="B60" s="1">
-        <v>43592.770833333299</v>
-      </c>
-      <c r="C60" s="1">
-        <v>43593.708333333336</v>
-      </c>
-      <c r="D60">
-        <v>3.5</v>
-      </c>
-      <c r="E60" s="22"/>
-      <c r="F60" s="26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>26</v>
-      </c>
-      <c r="E61" s="22">
-        <v>0.25</v>
       </c>
       <c r="F61" s="26" t="b">
         <v>1</v>
@@ -1876,24 +1864,44 @@
       <c r="A62" t="s">
         <v>26</v>
       </c>
-      <c r="E62" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="F62" s="5" t="b">
+      <c r="B62" s="1">
+        <v>43586</v>
+      </c>
+      <c r="C62" s="1">
+        <v>43592.770833333299</v>
+      </c>
+      <c r="D62">
+        <v>4.25</v>
+      </c>
+      <c r="E62" s="22"/>
+      <c r="F62" s="26" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>19</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B63" s="1">
+        <v>43592.770833333299</v>
+      </c>
+      <c r="C63" s="1">
+        <v>43593.708333333336</v>
+      </c>
+      <c r="D63">
+        <v>3.5</v>
+      </c>
+      <c r="E63" s="22"/>
       <c r="F63" s="26" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>20</v>
+        <v>26</v>
+      </c>
+      <c r="E64" s="22">
+        <v>0.25</v>
       </c>
       <c r="F64" s="26" t="b">
         <v>1</v>
@@ -1901,55 +1909,64 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>25</v>
-      </c>
-      <c r="F65" s="26" t="b">
+        <v>26</v>
+      </c>
+      <c r="E65" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="F65" s="5" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>25</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>81</v>
+        <v>19</v>
+      </c>
+      <c r="F66" s="26" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>20</v>
+      </c>
+      <c r="F67" s="26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>25</v>
+      </c>
+      <c r="F68" s="26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>25</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
         <v>4</v>
       </c>
-      <c r="B67" s="8">
+      <c r="B70" s="8">
         <v>43647.659722222219</v>
       </c>
-      <c r="C67" s="8">
+      <c r="C70" s="8">
         <v>43739</v>
       </c>
-      <c r="D67">
+      <c r="D70">
         <v>-0.15</v>
       </c>
-      <c r="E67"/>
-      <c r="F67" s="26" t="b">
+      <c r="E70"/>
+      <c r="F70" s="26" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B68"/>
-      <c r="C68"/>
-      <c r="E68"/>
-      <c r="F68"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B69"/>
-      <c r="C69"/>
-      <c r="E69"/>
-      <c r="F69"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B70"/>
-      <c r="C70"/>
-      <c r="E70"/>
-      <c r="F70"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B71"/>
@@ -2749,8 +2766,26 @@
       <c r="E203"/>
       <c r="F203"/>
     </row>
+    <row r="204" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B204"/>
+      <c r="C204"/>
+      <c r="E204"/>
+      <c r="F204"/>
+    </row>
+    <row r="205" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B205"/>
+      <c r="C205"/>
+      <c r="E205"/>
+      <c r="F205"/>
+    </row>
+    <row r="206" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B206"/>
+      <c r="C206"/>
+      <c r="E206"/>
+      <c r="F206"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G67">
+  <autoFilter ref="A1:G70">
     <sortState ref="A2:G58">
       <sortCondition ref="A2:A58"/>
       <sortCondition ref="B2:B58"/>
@@ -2766,11 +2801,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFC1341"/>
+  <dimension ref="A1:XFC1348"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A380" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D389" sqref="D389"/>
+      <pane ySplit="1" topLeftCell="A377" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D394" sqref="D394"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4501,7 +4536,7 @@
         <v>43648.541666666664</v>
       </c>
       <c r="D119" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="120" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -5059,7 +5094,7 @@
         <v>43665.177083333336</v>
       </c>
       <c r="D158" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F158" s="8"/>
       <c r="G158" s="8"/>
@@ -13263,7 +13298,7 @@
         <v>43666.177083333336</v>
       </c>
       <c r="D159" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="160" spans="1:1023 1026:2047 2050:3071 3074:4095 4098:5119 5122:6143 6146:7167 7170:8191 8194:9215 9218:10239 10242:11263 11266:12287 12290:13311 13314:14335 14338:15359 15362:16383" x14ac:dyDescent="0.3">
@@ -13861,7 +13896,7 @@
         <v>43671</v>
       </c>
       <c r="D201" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="202" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -28805,132 +28840,124 @@
       <c r="F387" s="8"/>
       <c r="G387" s="8"/>
     </row>
-    <row r="388" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A388" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B388" s="8">
+        <v>43637.520833333336</v>
+      </c>
+      <c r="C388" s="8">
+        <v>43641.538194444445</v>
+      </c>
+      <c r="D388" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F388" s="8"/>
+      <c r="G388" s="8"/>
+    </row>
+    <row r="389" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A389" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B389" s="8">
+        <v>43644.135416666664</v>
+      </c>
+      <c r="C389" s="8">
+        <v>43644.21875</v>
+      </c>
+      <c r="D389" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F389" s="8"/>
+      <c r="G389" s="8"/>
+    </row>
+    <row r="390" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A390" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B390" s="8">
+        <v>43644.572916666664</v>
+      </c>
+      <c r="C390" s="8">
+        <v>43647.489583333336</v>
+      </c>
+      <c r="D390" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E390" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="F390" s="8"/>
+      <c r="G390" s="8"/>
+    </row>
+    <row r="391" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A391" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B391" s="8">
+        <v>43655.552083333336</v>
+      </c>
+      <c r="C391" s="8">
         <v>43661.5625</v>
       </c>
-      <c r="C388" s="8">
-        <v>43661.604166666664</v>
-      </c>
-      <c r="D388" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E388" s="7"/>
-    </row>
-    <row r="389" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A389" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B389" s="8">
-        <v>43619</v>
-      </c>
-      <c r="C389" s="8">
-        <v>43619.125</v>
-      </c>
-      <c r="D389" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E389" s="7"/>
-    </row>
-    <row r="390" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A390" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B390" s="8">
-        <v>43633.083333333336</v>
-      </c>
-      <c r="C390" s="8">
-        <v>43633.458333333336</v>
-      </c>
-      <c r="D390" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E390" s="7"/>
-    </row>
-    <row r="391" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A391" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B391" s="8">
-        <v>43637</v>
-      </c>
-      <c r="C391" s="8">
-        <v>43641.541666666664</v>
-      </c>
       <c r="D391" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E391" s="7"/>
+        <v>124</v>
+      </c>
+      <c r="E391" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="F391" s="8"/>
+      <c r="G391" s="8"/>
     </row>
     <row r="392" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A392" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B392" s="8">
-        <v>43643.291666666664</v>
+        <v>43661.5625</v>
       </c>
       <c r="C392" s="8">
-        <v>43643.666666666664</v>
+        <v>43661.604166666664</v>
       </c>
       <c r="D392" s="7" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="E392" s="7"/>
     </row>
-    <row r="393" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A393" s="3" t="s">
-        <v>46</v>
+    <row r="393" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A393" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="B393" s="8">
-        <v>43644.229166666664</v>
+        <v>43668.784722222219</v>
       </c>
       <c r="C393" s="8">
-        <v>43644.583333333336</v>
+        <v>43669.243055555555</v>
       </c>
       <c r="D393" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E393" s="7"/>
-    </row>
-    <row r="394" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A394" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B394" s="8">
-        <v>43645.21875</v>
-      </c>
-      <c r="C394" s="8">
-        <v>43645.5625</v>
-      </c>
-      <c r="D394" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E394" s="7"/>
-    </row>
-    <row r="395" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A395" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B395" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D395" s="7"/>
-      <c r="E395" s="7" t="s">
-        <v>51</v>
-      </c>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="394" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A394" s="3"/>
+      <c r="B394" s="8"/>
+      <c r="C394" s="8"/>
+    </row>
+    <row r="395" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A395" s="3"/>
+      <c r="B395" s="8"/>
+      <c r="C395" s="8"/>
     </row>
     <row r="396" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A396" s="3" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="B396" s="8">
-        <v>43591.375</v>
+        <v>43619</v>
       </c>
       <c r="C396" s="8">
-        <v>43592.458333333336</v>
+        <v>43619.125</v>
       </c>
       <c r="D396" s="7" t="s">
         <v>47</v>
@@ -28939,106 +28966,103 @@
     </row>
     <row r="397" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A397" s="3" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="B397" s="8">
-        <v>43592.125</v>
+        <v>43633.083333333336</v>
       </c>
       <c r="C397" s="8">
-        <v>43594.416666666664</v>
+        <v>43633.458333333336</v>
       </c>
       <c r="D397" s="7" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="E397" s="7"/>
     </row>
     <row r="398" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A398" s="3" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="B398" s="8">
-        <v>43595.291666666664</v>
+        <v>43637</v>
       </c>
       <c r="C398" s="8">
-        <v>43595.416666666664</v>
+        <v>43641.541666666664</v>
       </c>
       <c r="D398" s="7" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="E398" s="7"/>
     </row>
     <row r="399" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A399" s="3" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="B399" s="8">
-        <v>43596.319444444445</v>
+        <v>43643.291666666664</v>
       </c>
       <c r="C399" s="8">
-        <v>43596.947916666664</v>
+        <v>43643.666666666664</v>
       </c>
       <c r="D399" s="7" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="E399" s="7"/>
     </row>
     <row r="400" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A400" s="3" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="B400" s="8">
-        <v>43601.333333333336</v>
+        <v>43644.229166666664</v>
       </c>
       <c r="C400" s="8">
-        <v>43601.854166666664</v>
+        <v>43644.583333333336</v>
       </c>
       <c r="D400" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E400" s="3"/>
+        <v>85</v>
+      </c>
+      <c r="E400" s="7"/>
     </row>
     <row r="401" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A401" s="3" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="B401" s="8">
-        <v>43604.083333333336</v>
+        <v>43645.21875</v>
       </c>
       <c r="C401" s="8">
-        <v>43605.1875</v>
+        <v>43645.5625</v>
       </c>
       <c r="D401" s="7" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="E401" s="7"/>
     </row>
     <row r="402" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A402" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B402" s="8">
-        <v>43604.083333333336</v>
-      </c>
-      <c r="C402" s="8">
-        <v>43633.6875</v>
-      </c>
-      <c r="D402" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E402" s="7"/>
+        <v>46</v>
+      </c>
+      <c r="B402" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D402" s="7"/>
+      <c r="E402" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="403" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A403" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B403" s="8">
-        <v>43605.190972222219</v>
+        <v>43591.375</v>
       </c>
       <c r="C403" s="8">
-        <v>43616.999305555553</v>
+        <v>43592.458333333336</v>
       </c>
       <c r="D403" s="7" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="E403" s="7"/>
     </row>
@@ -29047,40 +29071,40 @@
         <v>18</v>
       </c>
       <c r="B404" s="8">
-        <v>43637.270833333336</v>
+        <v>43592.125</v>
       </c>
       <c r="C404" s="8">
-        <v>43605.3125</v>
+        <v>43594.416666666664</v>
       </c>
       <c r="D404" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E404" s="7"/>
+    </row>
+    <row r="405" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A405" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B405" s="8">
+        <v>43595.291666666664</v>
+      </c>
+      <c r="C405" s="8">
+        <v>43595.416666666664</v>
+      </c>
+      <c r="D405" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E404" s="7"/>
-    </row>
-    <row r="405" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A405" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B405" s="8">
-        <v>43575</v>
-      </c>
-      <c r="C405" s="8">
-        <v>43593.75</v>
-      </c>
-      <c r="D405" s="7" t="s">
-        <v>76</v>
-      </c>
       <c r="E405" s="7"/>
     </row>
     <row r="406" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A406" s="7" t="s">
-        <v>26</v>
+      <c r="A406" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="B406" s="8">
-        <v>43594.965277777781</v>
+        <v>43596.319444444445</v>
       </c>
       <c r="C406" s="8">
-        <v>43595.375</v>
+        <v>43596.947916666664</v>
       </c>
       <c r="D406" s="7" t="s">
         <v>47</v>
@@ -29088,29 +29112,29 @@
       <c r="E406" s="7"/>
     </row>
     <row r="407" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A407" s="7" t="s">
-        <v>26</v>
+      <c r="A407" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="B407" s="8">
-        <v>43596.395833333336</v>
+        <v>43601.333333333336</v>
       </c>
       <c r="C407" s="8">
-        <v>43596.517361111109</v>
+        <v>43601.854166666664</v>
       </c>
       <c r="D407" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E407" s="7"/>
+      <c r="E407" s="3"/>
     </row>
     <row r="408" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A408" s="3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B408" s="8">
-        <v>43601.420138888891</v>
+        <v>43604.083333333336</v>
       </c>
       <c r="C408" s="8">
-        <v>43601.604166666664</v>
+        <v>43605.1875</v>
       </c>
       <c r="D408" s="7" t="s">
         <v>47</v>
@@ -29119,43 +29143,43 @@
     </row>
     <row r="409" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A409" s="3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B409" s="8">
-        <v>43604.4375</v>
+        <v>43604.083333333336</v>
       </c>
       <c r="C409" s="8">
-        <v>43604.638888888891</v>
+        <v>43633.6875</v>
       </c>
       <c r="D409" s="7" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="E409" s="7"/>
     </row>
     <row r="410" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A410" s="3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B410" s="8">
-        <v>43604.875</v>
+        <v>43605.190972222219</v>
       </c>
       <c r="C410" s="8">
-        <v>43605.569444444445</v>
+        <v>43616.999305555553</v>
       </c>
       <c r="D410" s="7" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="E410" s="7"/>
     </row>
     <row r="411" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A411" s="3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B411" s="8">
-        <v>43607.239583333336</v>
+        <v>43637.270833333336</v>
       </c>
       <c r="C411" s="8">
-        <v>43607.354166666664</v>
+        <v>43605.3125</v>
       </c>
       <c r="D411" s="7" t="s">
         <v>47</v>
@@ -29163,29 +29187,29 @@
       <c r="E411" s="7"/>
     </row>
     <row r="412" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A412" s="3" t="s">
+      <c r="A412" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B412" s="16">
-        <v>43611.885416666664</v>
-      </c>
-      <c r="C412" s="16">
-        <v>43612.34375</v>
+      <c r="B412" s="8">
+        <v>43575</v>
+      </c>
+      <c r="C412" s="8">
+        <v>43593.75</v>
       </c>
       <c r="D412" s="7" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="E412" s="7"/>
     </row>
     <row r="413" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A413" s="3" t="s">
+      <c r="A413" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B413" s="16">
-        <v>43637.208333333336</v>
-      </c>
-      <c r="C413" s="16">
-        <v>43637.416666666664</v>
+      <c r="B413" s="8">
+        <v>43594.965277777781</v>
+      </c>
+      <c r="C413" s="8">
+        <v>43595.375</v>
       </c>
       <c r="D413" s="7" t="s">
         <v>47</v>
@@ -29194,13 +29218,13 @@
     </row>
     <row r="414" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A414" s="7" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B414" s="8">
-        <v>43591.333333333336</v>
+        <v>43596.395833333336</v>
       </c>
       <c r="C414" s="8">
-        <v>43591.479166666664</v>
+        <v>43596.517361111109</v>
       </c>
       <c r="D414" s="7" t="s">
         <v>47</v>
@@ -29208,14 +29232,14 @@
       <c r="E414" s="7"/>
     </row>
     <row r="415" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A415" s="7" t="s">
-        <v>19</v>
+      <c r="A415" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B415" s="8">
-        <v>43592.173611111109</v>
+        <v>43601.420138888891</v>
       </c>
       <c r="C415" s="8">
-        <v>43592.288194444445</v>
+        <v>43601.604166666664</v>
       </c>
       <c r="D415" s="7" t="s">
         <v>47</v>
@@ -29223,14 +29247,14 @@
       <c r="E415" s="7"/>
     </row>
     <row r="416" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A416" s="7" t="s">
-        <v>19</v>
+      <c r="A416" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B416" s="8">
-        <v>43595.041666666664</v>
+        <v>43604.4375</v>
       </c>
       <c r="C416" s="8">
-        <v>43595.322916666664</v>
+        <v>43604.638888888891</v>
       </c>
       <c r="D416" s="7" t="s">
         <v>47</v>
@@ -29238,14 +29262,14 @@
       <c r="E416" s="7"/>
     </row>
     <row r="417" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A417" s="7" t="s">
-        <v>19</v>
+      <c r="A417" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B417" s="8">
-        <v>43596.270833333336</v>
+        <v>43604.875</v>
       </c>
       <c r="C417" s="8">
-        <v>43596.534722222219</v>
+        <v>43605.569444444445</v>
       </c>
       <c r="D417" s="7" t="s">
         <v>47</v>
@@ -29253,14 +29277,14 @@
       <c r="E417" s="7"/>
     </row>
     <row r="418" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A418" s="7" t="s">
-        <v>19</v>
+      <c r="A418" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B418" s="8">
-        <v>43601.40625</v>
+        <v>43607.239583333336</v>
       </c>
       <c r="C418" s="8">
-        <v>43601.565972222219</v>
+        <v>43607.354166666664</v>
       </c>
       <c r="D418" s="7" t="s">
         <v>47</v>
@@ -29268,14 +29292,14 @@
       <c r="E418" s="7"/>
     </row>
     <row r="419" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A419" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B419" s="8">
-        <v>43604.416666666664</v>
-      </c>
-      <c r="C419" s="8">
-        <v>43605.368055555555</v>
+      <c r="A419" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B419" s="16">
+        <v>43611.885416666664</v>
+      </c>
+      <c r="C419" s="16">
+        <v>43612.34375</v>
       </c>
       <c r="D419" s="7" t="s">
         <v>47</v>
@@ -29283,14 +29307,14 @@
       <c r="E419" s="7"/>
     </row>
     <row r="420" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A420" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B420" s="8">
-        <v>43606.951388888891</v>
-      </c>
-      <c r="C420" s="8">
-        <v>43607.875</v>
+      <c r="A420" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B420" s="16">
+        <v>43637.208333333336</v>
+      </c>
+      <c r="C420" s="16">
+        <v>43637.416666666664</v>
       </c>
       <c r="D420" s="7" t="s">
         <v>47</v>
@@ -29302,10 +29326,10 @@
         <v>19</v>
       </c>
       <c r="B421" s="8">
-        <v>43611.9375</v>
+        <v>43591.333333333336</v>
       </c>
       <c r="C421" s="8">
-        <v>43612.111111111109</v>
+        <v>43591.479166666664</v>
       </c>
       <c r="D421" s="7" t="s">
         <v>47</v>
@@ -29314,13 +29338,13 @@
     </row>
     <row r="422" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A422" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B422" s="8">
-        <v>43591.409722222219</v>
+        <v>43592.173611111109</v>
       </c>
       <c r="C422" s="8">
-        <v>43592.583333333336</v>
+        <v>43592.288194444445</v>
       </c>
       <c r="D422" s="7" t="s">
         <v>47</v>
@@ -29329,13 +29353,13 @@
     </row>
     <row r="423" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A423" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B423" s="8">
-        <v>43595.194444444445</v>
+        <v>43595.041666666664</v>
       </c>
       <c r="C423" s="8">
-        <v>43595.4375</v>
+        <v>43595.322916666664</v>
       </c>
       <c r="D423" s="7" t="s">
         <v>47</v>
@@ -29344,13 +29368,13 @@
     </row>
     <row r="424" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A424" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B424" s="8">
-        <v>43595.260416666664</v>
+        <v>43596.270833333336</v>
       </c>
       <c r="C424" s="8">
-        <v>43594.875</v>
+        <v>43596.534722222219</v>
       </c>
       <c r="D424" s="7" t="s">
         <v>47</v>
@@ -29359,13 +29383,13 @@
     </row>
     <row r="425" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A425" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B425" s="8">
-        <v>43596.340277777781</v>
+        <v>43601.40625</v>
       </c>
       <c r="C425" s="8">
-        <v>43596.895833333336</v>
+        <v>43601.565972222219</v>
       </c>
       <c r="D425" s="7" t="s">
         <v>47</v>
@@ -29374,13 +29398,13 @@
     </row>
     <row r="426" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A426" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B426" s="8">
-        <v>43601.440972222219</v>
+        <v>43604.416666666664</v>
       </c>
       <c r="C426" s="8">
-        <v>43601.822916666664</v>
+        <v>43605.368055555555</v>
       </c>
       <c r="D426" s="7" t="s">
         <v>47</v>
@@ -29389,13 +29413,13 @@
     </row>
     <row r="427" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A427" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B427" s="8">
-        <v>43604.440972222219</v>
+        <v>43606.951388888891</v>
       </c>
       <c r="C427" s="8">
-        <v>43608.708333333336</v>
+        <v>43607.875</v>
       </c>
       <c r="D427" s="7" t="s">
         <v>47</v>
@@ -29404,13 +29428,13 @@
     </row>
     <row r="428" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A428" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B428" s="8">
-        <v>43610.291666666664</v>
+        <v>43611.9375</v>
       </c>
       <c r="C428" s="8">
-        <v>43612.25</v>
+        <v>43612.111111111109</v>
       </c>
       <c r="D428" s="7" t="s">
         <v>47</v>
@@ -29422,10 +29446,10 @@
         <v>20</v>
       </c>
       <c r="B429" s="8">
-        <v>43633.583333333336</v>
+        <v>43591.409722222219</v>
       </c>
       <c r="C429" s="8">
-        <v>43633.833333333336</v>
+        <v>43592.583333333336</v>
       </c>
       <c r="D429" s="7" t="s">
         <v>47</v>
@@ -29437,10 +29461,10 @@
         <v>20</v>
       </c>
       <c r="B430" s="8">
-        <v>43637.104166666664</v>
+        <v>43595.194444444445</v>
       </c>
       <c r="C430" s="8">
-        <v>43637.791666666664</v>
+        <v>43595.4375</v>
       </c>
       <c r="D430" s="7" t="s">
         <v>47</v>
@@ -29452,25 +29476,25 @@
         <v>20</v>
       </c>
       <c r="B431" s="8">
-        <v>43646</v>
+        <v>43595.260416666664</v>
       </c>
       <c r="C431" s="8">
-        <v>43646.020833333336</v>
+        <v>43594.875</v>
       </c>
       <c r="D431" s="7" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="E431" s="7"/>
     </row>
     <row r="432" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A432" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B432" s="8">
-        <v>43591.375</v>
+        <v>43596.340277777781</v>
       </c>
       <c r="C432" s="8">
-        <v>43591.78125</v>
+        <v>43596.895833333336</v>
       </c>
       <c r="D432" s="7" t="s">
         <v>47</v>
@@ -29479,13 +29503,13 @@
     </row>
     <row r="433" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A433" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B433" s="8">
-        <v>43592.166666666664</v>
+        <v>43601.440972222219</v>
       </c>
       <c r="C433" s="8">
-        <v>43592.579861111109</v>
+        <v>43601.822916666664</v>
       </c>
       <c r="D433" s="7" t="s">
         <v>47</v>
@@ -29494,13 +29518,13 @@
     </row>
     <row r="434" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A434" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B434" s="8">
-        <v>43595.194444444445</v>
+        <v>43604.440972222219</v>
       </c>
       <c r="C434" s="8">
-        <v>43595.4375</v>
+        <v>43608.708333333336</v>
       </c>
       <c r="D434" s="7" t="s">
         <v>47</v>
@@ -29509,13 +29533,13 @@
     </row>
     <row r="435" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A435" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B435" s="8">
-        <v>43595.260416666664</v>
+        <v>43610.291666666664</v>
       </c>
       <c r="C435" s="8">
-        <v>43594.875</v>
+        <v>43612.25</v>
       </c>
       <c r="D435" s="7" t="s">
         <v>47</v>
@@ -29524,13 +29548,13 @@
     </row>
     <row r="436" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A436" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B436" s="8">
-        <v>43596.340277777781</v>
+        <v>43633.583333333336</v>
       </c>
       <c r="C436" s="8">
-        <v>43596.895833333336</v>
+        <v>43633.833333333336</v>
       </c>
       <c r="D436" s="7" t="s">
         <v>47</v>
@@ -29539,13 +29563,13 @@
     </row>
     <row r="437" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A437" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B437" s="8">
-        <v>43601.388888888891</v>
+        <v>43637.104166666664</v>
       </c>
       <c r="C437" s="8">
-        <v>43601.822916666664</v>
+        <v>43637.791666666664</v>
       </c>
       <c r="D437" s="7" t="s">
         <v>47</v>
@@ -29554,16 +29578,16 @@
     </row>
     <row r="438" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A438" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B438" s="8">
-        <v>43604.350694444445</v>
+        <v>43646</v>
       </c>
       <c r="C438" s="8">
-        <v>43608.708333333336</v>
+        <v>43646.020833333336</v>
       </c>
       <c r="D438" s="7" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="E438" s="7"/>
     </row>
@@ -29572,10 +29596,10 @@
         <v>25</v>
       </c>
       <c r="B439" s="8">
-        <v>43611.892361111109</v>
+        <v>43591.375</v>
       </c>
       <c r="C439" s="8">
-        <v>43612.25</v>
+        <v>43591.78125</v>
       </c>
       <c r="D439" s="7" t="s">
         <v>47</v>
@@ -29587,13 +29611,13 @@
         <v>25</v>
       </c>
       <c r="B440" s="8">
-        <v>43616.208333333336</v>
+        <v>43592.166666666664</v>
       </c>
       <c r="C440" s="8">
-        <v>43616.701388888891</v>
+        <v>43592.579861111109</v>
       </c>
       <c r="D440" s="7" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="E440" s="7"/>
     </row>
@@ -29602,13 +29626,13 @@
         <v>25</v>
       </c>
       <c r="B441" s="8">
-        <v>43616.208333333336</v>
+        <v>43595.194444444445</v>
       </c>
       <c r="C441" s="8">
-        <v>43616.701388888891</v>
+        <v>43595.4375</v>
       </c>
       <c r="D441" s="7" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="E441" s="7"/>
     </row>
@@ -29617,10 +29641,10 @@
         <v>25</v>
       </c>
       <c r="B442" s="8">
-        <v>43633.583333333336</v>
+        <v>43595.260416666664</v>
       </c>
       <c r="C442" s="8">
-        <v>43633.791666666664</v>
+        <v>43594.875</v>
       </c>
       <c r="D442" s="7" t="s">
         <v>47</v>
@@ -29632,10 +29656,10 @@
         <v>25</v>
       </c>
       <c r="B443" s="8">
-        <v>43637.104166666664</v>
+        <v>43596.340277777781</v>
       </c>
       <c r="C443" s="8">
-        <v>43637.791666666664</v>
+        <v>43596.895833333336</v>
       </c>
       <c r="D443" s="7" t="s">
         <v>47</v>
@@ -29643,295 +29667,302 @@
       <c r="E443" s="7"/>
     </row>
     <row r="444" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A444" s="3" t="s">
+      <c r="A444" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B444" s="8">
+        <v>43601.388888888891</v>
+      </c>
+      <c r="C444" s="8">
+        <v>43601.822916666664</v>
+      </c>
+      <c r="D444" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E444" s="7"/>
+    </row>
+    <row r="445" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A445" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B445" s="8">
+        <v>43604.350694444445</v>
+      </c>
+      <c r="C445" s="8">
+        <v>43608.708333333336</v>
+      </c>
+      <c r="D445" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E445" s="7"/>
+    </row>
+    <row r="446" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A446" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B446" s="8">
+        <v>43611.892361111109</v>
+      </c>
+      <c r="C446" s="8">
+        <v>43612.25</v>
+      </c>
+      <c r="D446" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E446" s="7"/>
+    </row>
+    <row r="447" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A447" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B447" s="8">
+        <v>43616.208333333336</v>
+      </c>
+      <c r="C447" s="8">
+        <v>43616.701388888891</v>
+      </c>
+      <c r="D447" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E447" s="7"/>
+    </row>
+    <row r="448" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A448" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B448" s="8">
+        <v>43616.208333333336</v>
+      </c>
+      <c r="C448" s="8">
+        <v>43616.701388888891</v>
+      </c>
+      <c r="D448" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E448" s="7"/>
+    </row>
+    <row r="449" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A449" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B449" s="8">
+        <v>43633.583333333336</v>
+      </c>
+      <c r="C449" s="8">
+        <v>43633.791666666664</v>
+      </c>
+      <c r="D449" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E449" s="7"/>
+    </row>
+    <row r="450" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A450" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B450" s="8">
+        <v>43637.104166666664</v>
+      </c>
+      <c r="C450" s="8">
+        <v>43637.791666666664</v>
+      </c>
+      <c r="D450" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E450" s="7"/>
+    </row>
+    <row r="451" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A451" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B444" s="8">
+      <c r="B451" s="8">
         <v>43669.013888888891</v>
       </c>
-      <c r="C444" s="8">
+      <c r="C451" s="8">
         <v>43669.182638888888</v>
       </c>
-      <c r="D444" s="7" t="s">
+      <c r="D451" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E444" s="7"/>
-    </row>
-    <row r="445" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A445" t="s">
+      <c r="E451" s="7"/>
+    </row>
+    <row r="452" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A452" t="s">
         <v>7</v>
       </c>
-      <c r="B445" s="8">
+      <c r="B452" s="8">
         <v>43670.631944444445</v>
       </c>
-      <c r="C445" s="8">
+      <c r="C452" s="8">
         <v>43670.788194444445</v>
       </c>
-      <c r="D445" t="s">
+      <c r="D452" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="446" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A446" t="s">
+    <row r="453" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A453" t="s">
         <v>7</v>
       </c>
-      <c r="B446" s="8">
+      <c r="B453" s="8">
         <v>43674.638888888891</v>
       </c>
-      <c r="C446" s="8">
+      <c r="C453" s="8">
         <v>43674.791666666664</v>
       </c>
-      <c r="D446" t="s">
+      <c r="D453" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="447" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A447" t="s">
+    <row r="454" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A454" t="s">
         <v>7</v>
       </c>
-      <c r="B447" s="8">
+      <c r="B454" s="8">
         <v>43675.020833333336</v>
       </c>
-      <c r="C447" s="8">
+      <c r="C454" s="8">
         <v>43675.180555555555</v>
       </c>
-      <c r="D447" t="s">
+      <c r="D454" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="448" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A448" t="s">
+    <row r="455" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A455" t="s">
         <v>7</v>
       </c>
-      <c r="B448" s="8">
+      <c r="B455" s="8">
         <v>43676.642361111109</v>
       </c>
-      <c r="C448" s="8">
+      <c r="C455" s="8">
         <v>43676.795138888891</v>
       </c>
-      <c r="D448" t="s">
+      <c r="D455" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="449" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A449" t="s">
+    <row r="456" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A456" t="s">
         <v>7</v>
       </c>
-      <c r="B449" s="8">
+      <c r="B456" s="8">
         <v>43677.638888888891</v>
       </c>
-      <c r="C449" s="8">
+      <c r="C456" s="8">
         <v>43677.791666666664</v>
       </c>
-      <c r="D449" t="s">
+      <c r="D456" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="450" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A450" s="3" t="s">
+    <row r="457" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A457" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B450" s="8">
+      <c r="B457" s="8">
         <v>43649.229166666664</v>
       </c>
-      <c r="C450" s="8">
+      <c r="C457" s="8">
         <v>43651.916666666664</v>
       </c>
-      <c r="D450" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="451" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A451" s="3" t="s">
+      <c r="D457" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="458" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A458" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B451" s="8">
+      <c r="B458" s="8">
         <v>43664.972222222219</v>
       </c>
-      <c r="C451" s="8">
+      <c r="C458" s="8">
         <v>43671.9375</v>
       </c>
-      <c r="D451" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="452" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A452" s="3" t="s">
+      <c r="D458" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="459" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A459" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B452" s="8">
+      <c r="B459" s="8">
         <v>43647.697916666664</v>
       </c>
-      <c r="C452" s="8">
+      <c r="C459" s="8">
         <v>43648.583333333336</v>
       </c>
-      <c r="D452" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="453" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A453" s="3" t="s">
+      <c r="D459" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="460" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A460" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B453" s="8">
+      <c r="B460" s="8">
         <v>43654.802083333336</v>
       </c>
-      <c r="C453" s="8">
+      <c r="C460" s="8">
         <v>43657.770833333336</v>
       </c>
-      <c r="D453" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="454" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A454" s="3" t="s">
+      <c r="D460" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="461" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A461" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B454" s="8">
+      <c r="B461" s="8">
         <v>43670.85</v>
       </c>
-      <c r="C454" s="8">
+      <c r="C461" s="8">
         <v>43672.670138888891</v>
       </c>
-      <c r="D454" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="455" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A455" s="3" t="s">
+      <c r="D461" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="462" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A462" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B455" s="8">
+      <c r="B462" s="8">
         <v>43662.652777777781</v>
       </c>
-      <c r="C455" s="8">
+      <c r="C462" s="8">
         <v>43662.694444444445</v>
-      </c>
-      <c r="D455" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="456" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A456" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B456" s="8">
-        <v>43668.541666666664</v>
-      </c>
-      <c r="C456" s="8">
-        <v>43668.5625</v>
-      </c>
-      <c r="D456" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="457" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A457" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B457" s="8">
-        <v>43676.263888888891</v>
-      </c>
-      <c r="C457" s="8">
-        <v>43676.305555555555</v>
-      </c>
-      <c r="D457" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="458" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A458" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B458" s="8">
-        <v>43647.649305555555</v>
-      </c>
-      <c r="C458" s="8">
-        <v>43647.659722222219</v>
-      </c>
-      <c r="D458" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="459" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A459" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B459" s="33">
-        <v>43661.048611111109</v>
-      </c>
-      <c r="C459" s="8">
-        <v>43661.163194444445</v>
-      </c>
-      <c r="D459" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="460" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A460" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B460" s="8">
-        <v>43663.003472222219</v>
-      </c>
-      <c r="C460" s="8">
-        <v>43663.03125</v>
-      </c>
-      <c r="D460" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="461" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A461" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B461" s="8">
-        <v>43669.003472222219</v>
-      </c>
-      <c r="C461" s="8">
-        <v>43669.03125</v>
-      </c>
-      <c r="D461" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="462" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A462" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B462" s="8">
-        <v>43669.71875</v>
-      </c>
-      <c r="C462" s="8">
-        <v>43669.795138888891</v>
       </c>
       <c r="D462" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="463" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A463" s="3" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B463" s="8">
-        <v>43674.003472222219</v>
+        <v>43668.541666666664</v>
       </c>
       <c r="C463" s="8">
-        <v>43674.03125</v>
+        <v>43668.5625</v>
       </c>
       <c r="D463" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="464" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A464" s="3" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B464" s="8">
-        <v>43675.003472222219</v>
+        <v>43676.263888888891</v>
       </c>
       <c r="C464" s="8">
-        <v>43675.048611111109</v>
+        <v>43676.305555555555</v>
       </c>
       <c r="D464" s="7" t="s">
         <v>75</v>
@@ -29939,45 +29970,115 @@
     </row>
     <row r="465" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A465" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B465" s="8">
+        <v>43647.649305555555</v>
+      </c>
+      <c r="C465" s="8">
+        <v>43647.659722222219</v>
+      </c>
+      <c r="D465" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="466" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A466" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B465" s="8">
+      <c r="B466" s="33">
+        <v>43661.048611111109</v>
+      </c>
+      <c r="C466" s="8">
+        <v>43661.163194444445</v>
+      </c>
+      <c r="D466" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="467" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A467" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B467" s="8">
+        <v>43663.003472222219</v>
+      </c>
+      <c r="C467" s="8">
+        <v>43663.03125</v>
+      </c>
+      <c r="D467" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="468" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A468" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B468" s="8">
+        <v>43669.003472222219</v>
+      </c>
+      <c r="C468" s="8">
+        <v>43669.03125</v>
+      </c>
+      <c r="D468" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="469" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A469" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B469" s="8">
+        <v>43669.71875</v>
+      </c>
+      <c r="C469" s="8">
+        <v>43669.795138888891</v>
+      </c>
+      <c r="D469" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="470" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A470" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B470" s="8">
+        <v>43674.003472222219</v>
+      </c>
+      <c r="C470" s="8">
+        <v>43674.03125</v>
+      </c>
+      <c r="D470" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="471" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A471" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B471" s="8">
+        <v>43675.003472222219</v>
+      </c>
+      <c r="C471" s="8">
+        <v>43675.048611111109</v>
+      </c>
+      <c r="D471" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="472" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A472" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B472" s="8">
         <v>43676.003472222219</v>
       </c>
-      <c r="C465" s="8">
+      <c r="C472" s="8">
         <v>43676.03125</v>
       </c>
-      <c r="D465" s="7" t="s">
+      <c r="D472" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="466" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B466"/>
-      <c r="C466"/>
-    </row>
-    <row r="467" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B467"/>
-      <c r="C467"/>
-    </row>
-    <row r="468" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B468"/>
-      <c r="C468"/>
-    </row>
-    <row r="469" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B469"/>
-      <c r="C469"/>
-    </row>
-    <row r="470" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B470"/>
-      <c r="C470"/>
-    </row>
-    <row r="471" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B471"/>
-      <c r="C471"/>
-    </row>
-    <row r="472" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B472"/>
-      <c r="C472"/>
     </row>
     <row r="473" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B473"/>
@@ -33455,8 +33556,36 @@
       <c r="B1341"/>
       <c r="C1341"/>
     </row>
+    <row r="1342" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B1342"/>
+      <c r="C1342"/>
+    </row>
+    <row r="1343" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B1343"/>
+      <c r="C1343"/>
+    </row>
+    <row r="1344" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B1344"/>
+      <c r="C1344"/>
+    </row>
+    <row r="1345" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B1345"/>
+      <c r="C1345"/>
+    </row>
+    <row r="1346" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B1346"/>
+      <c r="C1346"/>
+    </row>
+    <row r="1347" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B1347"/>
+      <c r="C1347"/>
+    </row>
+    <row r="1348" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B1348"/>
+      <c r="C1348"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E465"/>
+  <autoFilter ref="A1:E472"/>
   <sortState ref="A2:E443">
     <sortCondition ref="A2:A443"/>
     <sortCondition ref="B2:B443"/>
@@ -33473,11 +33602,11 @@
   </sheetPr>
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="24.9" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -33500,10 +33629,10 @@
         <v>53</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -33515,7 +33644,7 @@
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>90</v>
@@ -33529,7 +33658,7 @@
         <v>90</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D3" s="32"/>
     </row>
@@ -33541,7 +33670,7 @@
         <v>90</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D4" s="32"/>
     </row>
@@ -33553,7 +33682,7 @@
         <v>90</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D5" s="32"/>
     </row>
@@ -33566,7 +33695,7 @@
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>90</v>
@@ -33581,10 +33710,10 @@
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -33596,10 +33725,10 @@
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -33610,7 +33739,7 @@
         <v>88</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D9" s="32"/>
     </row>
@@ -33623,10 +33752,10 @@
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -33637,7 +33766,7 @@
         <v>90</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D11" s="32"/>
     </row>
@@ -33649,7 +33778,7 @@
         <v>87</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D12" s="32"/>
     </row>
@@ -33661,7 +33790,7 @@
         <v>92</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D13" s="32"/>
     </row>
@@ -33674,10 +33803,10 @@
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>123</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -33685,10 +33814,10 @@
         <v>10</v>
       </c>
       <c r="B15" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>111</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>112</v>
       </c>
       <c r="D15" s="32"/>
     </row>
@@ -33700,7 +33829,7 @@
         <v>94</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D16" s="32"/>
     </row>
@@ -33712,7 +33841,7 @@
         <v>90</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D17" s="32"/>
     </row>
@@ -33721,10 +33850,10 @@
         <v>40</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D18" s="32"/>
     </row>
@@ -33736,7 +33865,7 @@
         <v>106</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D19" s="32"/>
     </row>
@@ -33748,7 +33877,7 @@
         <v>96</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D20" s="32"/>
     </row>
@@ -33770,7 +33899,7 @@
         <v>97</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D22" s="32"/>
     </row>
@@ -33792,7 +33921,7 @@
         <v>99</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D24" s="32"/>
     </row>
@@ -33804,7 +33933,7 @@
         <v>100</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D25" s="32"/>
     </row>
@@ -33816,7 +33945,7 @@
         <v>101</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D26" s="32"/>
     </row>
@@ -33828,7 +33957,7 @@
         <v>90</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D27" s="32"/>
     </row>
@@ -33840,7 +33969,7 @@
         <v>102</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D28" s="32"/>
     </row>
@@ -33852,7 +33981,7 @@
         <v>90</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D29" s="32"/>
     </row>
@@ -33864,7 +33993,7 @@
         <v>103</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D30" s="32"/>
     </row>
@@ -33876,7 +34005,7 @@
         <v>104</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D31" s="32"/>
     </row>
@@ -33898,7 +34027,7 @@
         <v>90</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D33" s="32"/>
     </row>
@@ -33910,12 +34039,12 @@
       <c r="C34" s="11"/>
       <c r="D34" s="32"/>
     </row>
-    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
         <v>45</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="32"/>
@@ -33928,7 +34057,7 @@
         <v>90</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D36" s="32"/>
     </row>
@@ -33937,7 +34066,7 @@
         <v>18</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="32"/>
@@ -33950,7 +34079,7 @@
         <v>90</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D38" s="32"/>
     </row>
@@ -33959,7 +34088,7 @@
         <v>19</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="32"/>
@@ -33969,7 +34098,7 @@
         <v>20</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="32"/>
@@ -33982,7 +34111,7 @@
         <v>90</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D41" s="32"/>
     </row>

</xml_diff>

<commit_message>
updates to deliverabel pivot tables
</commit_message>
<xml_diff>
--- a/2 - Flow output Excel files - working drafts/Data Output 07_31_2019/Offsets and Clip times 07_31_2019.xlsx
+++ b/2 - Flow output Excel files - working drafts/Data Output 07_31_2019/Offsets and Clip times 07_31_2019.xlsx
@@ -592,7 +592,7 @@
         <xdr:cNvPr id="2" name="EsriDoNotEdit">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33597,7 +33597,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:E41"/>
@@ -33606,7 +33606,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B37" sqref="B37"/>
+      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="24.9" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -33650,7 +33650,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="28" t="s">
         <v>5</v>
       </c>
@@ -33662,7 +33662,7 @@
       </c>
       <c r="D3" s="32"/>
     </row>
-    <row r="4" spans="1:5" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>29</v>
       </c>
@@ -33674,7 +33674,7 @@
       </c>
       <c r="D4" s="32"/>
     </row>
-    <row r="5" spans="1:5" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>24</v>
       </c>
@@ -33731,7 +33731,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>31</v>
       </c>
@@ -33758,7 +33758,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>42</v>
       </c>
@@ -33770,7 +33770,7 @@
       </c>
       <c r="D11" s="32"/>
     </row>
-    <row r="12" spans="1:5" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
         <v>50</v>
       </c>
@@ -33782,7 +33782,7 @@
       </c>
       <c r="D12" s="32"/>
     </row>
-    <row r="13" spans="1:5" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="28" t="s">
         <v>8</v>
       </c>
@@ -33809,7 +33809,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="28" t="s">
         <v>10</v>
       </c>
@@ -33821,7 +33821,7 @@
       </c>
       <c r="D15" s="32"/>
     </row>
-    <row r="16" spans="1:5" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>11</v>
       </c>
@@ -33833,7 +33833,7 @@
       </c>
       <c r="D16" s="32"/>
     </row>
-    <row r="17" spans="1:4" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="28" t="s">
         <v>12</v>
       </c>
@@ -33845,7 +33845,7 @@
       </c>
       <c r="D17" s="32"/>
     </row>
-    <row r="18" spans="1:4" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>40</v>
       </c>
@@ -33857,7 +33857,7 @@
       </c>
       <c r="D18" s="32"/>
     </row>
-    <row r="19" spans="1:4" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>41</v>
       </c>
@@ -33869,7 +33869,7 @@
       </c>
       <c r="D19" s="32"/>
     </row>
-    <row r="20" spans="1:4" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="28" t="s">
         <v>13</v>
       </c>
@@ -33891,7 +33891,7 @@
       <c r="C21" s="11"/>
       <c r="D21" s="32"/>
     </row>
-    <row r="22" spans="1:4" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
         <v>14</v>
       </c>
@@ -33913,7 +33913,7 @@
       <c r="C23" s="11"/>
       <c r="D23" s="32"/>
     </row>
-    <row r="24" spans="1:4" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
         <v>16</v>
       </c>
@@ -33925,7 +33925,7 @@
       </c>
       <c r="D24" s="32"/>
     </row>
-    <row r="25" spans="1:4" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
         <v>32</v>
       </c>
@@ -33937,7 +33937,7 @@
       </c>
       <c r="D25" s="32"/>
     </row>
-    <row r="26" spans="1:4" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
         <v>17</v>
       </c>
@@ -33949,7 +33949,7 @@
       </c>
       <c r="D26" s="32"/>
     </row>
-    <row r="27" spans="1:4" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
         <v>33</v>
       </c>
@@ -33961,7 +33961,7 @@
       </c>
       <c r="D27" s="32"/>
     </row>
-    <row r="28" spans="1:4" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
         <v>34</v>
       </c>
@@ -33973,7 +33973,7 @@
       </c>
       <c r="D28" s="32"/>
     </row>
-    <row r="29" spans="1:4" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
         <v>35</v>
       </c>
@@ -33985,7 +33985,7 @@
       </c>
       <c r="D29" s="32"/>
     </row>
-    <row r="30" spans="1:4" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="11" t="s">
         <v>36</v>
       </c>
@@ -33997,7 +33997,7 @@
       </c>
       <c r="D30" s="32"/>
     </row>
-    <row r="31" spans="1:4" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="11" t="s">
         <v>37</v>
       </c>
@@ -34019,7 +34019,7 @@
       <c r="C32" s="11"/>
       <c r="D32" s="32"/>
     </row>
-    <row r="33" spans="1:4" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
         <v>39</v>
       </c>
@@ -34049,7 +34049,7 @@
       <c r="C35" s="11"/>
       <c r="D35" s="32"/>
     </row>
-    <row r="36" spans="1:4" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="11" t="s">
         <v>46</v>
       </c>
@@ -34071,7 +34071,7 @@
       <c r="C37" s="11"/>
       <c r="D37" s="32"/>
     </row>
-    <row r="38" spans="1:4" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="11" t="s">
         <v>26</v>
       </c>
@@ -34103,7 +34103,7 @@
       <c r="C40" s="11"/>
       <c r="D40" s="32"/>
     </row>
-    <row r="41" spans="1:4" ht="24.9" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="24.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="11" t="s">
         <v>25</v>
       </c>
@@ -34116,11 +34116,7 @@
       <c r="D41" s="32"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C41">
-    <filterColumn colId="2">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C41"/>
   <sortState ref="A2:A16">
     <sortCondition ref="A2:A16"/>
   </sortState>

</xml_diff>

<commit_message>
updating git attributes to see if we can diff xlsx files
</commit_message>
<xml_diff>
--- a/2 - Flow output Excel files - working drafts/Data Output 07_31_2019/Offsets and Clip times 07_31_2019.xlsx
+++ b/2 - Flow output Excel files - working drafts/Data Output 07_31_2019/Offsets and Clip times 07_31_2019.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="129">
   <si>
     <t>Site</t>
   </si>
@@ -414,6 +414,12 @@
   <si>
     <t>level spike on 7/15 same day as manual download. Looks like pattern of higher water temp with the pumping pattern. One period of data (7/9-7/15) was clipped out since it didn't match up with the game cam observations</t>
   </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>testing testing</t>
+  </si>
 </sst>
 </file>
 
@@ -592,7 +598,7 @@
         <xdr:cNvPr id="2" name="EsriDoNotEdit">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33600,13 +33606,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
+      <selection pane="bottomRight" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="24.9" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -34114,6 +34120,14 @@
         <v>111</v>
       </c>
       <c r="D41" s="32"/>
+    </row>
+    <row r="42" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>128</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C41"/>

</xml_diff>

<commit_message>
updated to initials on site completion
</commit_message>
<xml_diff>
--- a/2 - Flow output Excel files - working drafts/Data Output 07_31_2019/Offsets and Clip times 07_31_2019.xlsx
+++ b/2 - Flow output Excel files - working drafts/Data Output 07_31_2019/Offsets and Clip times 07_31_2019.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="9336" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="9336" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Offsets" sheetId="1" r:id="rId1"/>
@@ -277,9 +277,6 @@
     <t>removed probe to clean</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>Bad data-doesn't match with game cam</t>
   </si>
   <si>
@@ -336,6 +333,9 @@
   </si>
   <si>
     <t>Leaf Obstruction at crest of weir</t>
+  </si>
+  <si>
+    <t>AM</t>
   </si>
 </sst>
 </file>
@@ -509,7 +509,7 @@
         <xdr:cNvPr id="2" name="EsriDoNotEdit">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2724,7 +2724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFC1373"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B173" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -5273,7 +5273,7 @@
         <v>43636.938888888886</v>
       </c>
       <c r="D176" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="177" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -5287,7 +5287,7 @@
         <v>43638.563888888886</v>
       </c>
       <c r="D177" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="178" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -5301,7 +5301,7 @@
         <v>43639.355555555558</v>
       </c>
       <c r="D178" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="179" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -5315,7 +5315,7 @@
         <v>43640.109722222223</v>
       </c>
       <c r="D179" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="180" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -5329,7 +5329,7 @@
         <v>43644.943749999999</v>
       </c>
       <c r="D180" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="181" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -5343,7 +5343,7 @@
         <v>43653.038194444445</v>
       </c>
       <c r="D181" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="182" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -5357,7 +5357,7 @@
         <v>43654.954861111109</v>
       </c>
       <c r="D182" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="183" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -5371,7 +5371,7 @@
         <v>43663.472222222219</v>
       </c>
       <c r="D183" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="184" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -5748,7 +5748,7 @@
         <v>43620.5</v>
       </c>
       <c r="D218" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.3">
@@ -5777,7 +5777,7 @@
         <v>43661.510416666664</v>
       </c>
       <c r="D220" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="221" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -5791,10 +5791,10 @@
         <v>43591.513888888891</v>
       </c>
       <c r="D221" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E221" t="s">
         <v>88</v>
-      </c>
-      <c r="E221" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="222" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -19816,7 +19816,7 @@
         <v>43654.788194444445</v>
       </c>
       <c r="D343" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="344" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -20008,10 +20008,10 @@
         <v>43647.489583333336</v>
       </c>
       <c r="D356" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E356" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="E356" s="7" t="s">
-        <v>83</v>
       </c>
       <c r="F356" s="8"/>
       <c r="G356" s="8"/>
@@ -20027,10 +20027,10 @@
         <v>43661.5625</v>
       </c>
       <c r="D357" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E357" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="E357" s="7" t="s">
-        <v>83</v>
       </c>
       <c r="F357" s="8"/>
       <c r="G357" s="8"/>
@@ -20217,7 +20217,7 @@
         <v>43665.5625</v>
       </c>
       <c r="D370" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="371" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -20231,7 +20231,7 @@
         <v>43669.267361111109</v>
       </c>
       <c r="D371" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="372" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -20245,7 +20245,7 @@
         <v>43676.225694444445</v>
       </c>
       <c r="D372" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="373" spans="1:5" x14ac:dyDescent="0.3">
@@ -32908,11 +32908,11 @@
   </sheetPr>
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomRight" activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="24.9" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -33044,10 +33044,10 @@
         <v>12</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -33055,10 +33055,10 @@
         <v>40</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -33087,10 +33087,10 @@
         <v>14</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -33098,10 +33098,10 @@
         <v>15</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -33144,10 +33144,10 @@
         <v>35</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -33183,10 +33183,10 @@
         <v>44</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -33194,10 +33194,10 @@
         <v>45</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -33205,10 +33205,10 @@
         <v>46</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -33216,10 +33216,10 @@
         <v>18</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -33227,10 +33227,10 @@
         <v>26</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -33238,10 +33238,10 @@
         <v>19</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="24.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -33249,10 +33249,10 @@
         <v>20</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="24.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -33260,10 +33260,10 @@
         <v>25</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
preprocessing for August data
</commit_message>
<xml_diff>
--- a/2 - Flow output Excel files - working drafts/Data Output 07_31_2019/Offsets and Clip times 07_31_2019.xlsx
+++ b/2 - Flow output Excel files - working drafts/Data Output 07_31_2019/Offsets and Clip times 07_31_2019.xlsx
@@ -617,7 +617,7 @@
         <xdr:cNvPr id="2" name="EsriDoNotEdit">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33857,10 +33857,10 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:B37"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="24.9" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>